<commit_message>
Minor corrects to excel attachment
</commit_message>
<xml_diff>
--- a/TransferMateTC.xlsx
+++ b/TransferMateTC.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="42">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -218,7 +218,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -240,6 +240,27 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF00A933"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="134"/>
     </font>
     <font>
       <b val="true"/>
@@ -282,7 +303,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -306,8 +327,17 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -320,15 +350,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -344,31 +370,102 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="9">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Untitled1" xfId="20"/>
+    <cellStyle name="Untitled2" xfId="21"/>
+    <cellStyle name="Untitled3" xfId="22"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
       <font>
-        <color rgb="FFFF0000"/>
+        <name val="Calibri"/>
+        <charset val="134"/>
+        <family val="0"/>
+        <color rgb="FF00A933"/>
+        <sz val="13"/>
       </font>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF00B050"/>
+        <name val="Calibri"/>
+        <charset val="134"/>
+        <family val="0"/>
+        <color rgb="FFFF0000"/>
+        <sz val="11"/>
       </font>
     </dxf>
   </dxfs>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF00A933"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -379,22 +476,22 @@
   </sheetPr>
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F:F"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="74.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="22.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="22.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="20.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="43.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="37.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -413,7 +510,7 @@
       <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
@@ -427,207 +524,219 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="n">
+      <c r="A2" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="127.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="n">
+      <c r="A3" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="n">
+      <c r="A4" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="n">
+      <c r="A5" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="n">
+      <c r="A6" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="6" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="n">
+      <c r="A7" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="161.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="n">
+      <c r="A8" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="7" t="s">
+      <c r="F8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="I8" s="6" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>passed</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>failed</formula>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>